<commit_message>
screenshots for the readme.md
</commit_message>
<xml_diff>
--- a/projectDocs/ProjectLog.xlsx
+++ b/projectDocs/ProjectLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>GitHub fight</t>
+  </si>
+  <si>
+    <t>README.md</t>
   </si>
 </sst>
 </file>
@@ -632,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +686,7 @@
       </c>
       <c r="G2" s="4">
         <f>SUMPRODUCT(D2:D1000)</f>
-        <v>6.1250000000000027</v>
+        <v>6.2291666666666696</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1987,10 +1990,7 @@
         <f>SUMPRODUCT(D2:D61)</f>
         <v>3.2048611111111134</v>
       </c>
-      <c r="G61" s="4">
-        <f>SUMPRODUCT(D61:D1059)</f>
-        <v>2.9409722222222219</v>
-      </c>
+      <c r="G61" s="4"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
@@ -2312,7 +2312,7 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="D76" s="5">
-        <f t="shared" ref="D76:D91" si="1">C76-B76</f>
+        <f t="shared" ref="D76:D92" si="1">C76-B76</f>
         <v>9.3055555555555558E-2</v>
       </c>
       <c r="E76" t="s">
@@ -2660,6 +2660,20 @@
       <c r="B92" s="1">
         <v>0.64583333333333337</v>
       </c>
+      <c r="C92" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D92" s="5">
+        <f t="shared" si="1"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="E92" t="s">
+        <v>81</v>
+      </c>
+      <c r="F92" s="4">
+        <f>SUMPRODUCT(D2:D92)</f>
+        <v>5.6041666666666696</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D94" s="5">
@@ -2670,13 +2684,13 @@
       </c>
       <c r="F94" s="4">
         <f>SUMPRODUCT(D2:D94)</f>
-        <v>6.1250000000000027</v>
+        <v>6.2291666666666696</v>
       </c>
     </row>
     <row r="1048576" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D1048576" s="5">
         <f>SUM(D2:D1048575)</f>
-        <v>6.1250000000000027</v>
+        <v>6.2291666666666696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>